<commit_message>
Updating Guia and note-be
</commit_message>
<xml_diff>
--- a/Guia_fs2021.xlsx
+++ b/Guia_fs2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Bitacora" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,9 +16,10 @@
     <sheet name="Cors" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Heroku" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Heroku-App" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Folders" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Debbugging" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="MongoDB" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Heroku-Trouble" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Folders" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Debbugging" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="MongoDB" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="421">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -264,10 +265,16 @@
     <t xml:space="preserve">Backend conectado a una base de datos</t>
   </si>
   <si>
+    <t xml:space="preserve">Intermedio de pizza y otros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base de datos de la agenda telefónica, paso 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rama</t>
   </si>
   <si>
-    <t xml:space="preserve">Part3c-2-Notes-BackEndToMongoDB</t>
+    <t xml:space="preserve">Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</t>
   </si>
   <si>
     <t xml:space="preserve">Mensaje</t>
@@ -1259,6 +1266,12 @@
     <t xml:space="preserve">https://git.heroku.com/&lt;heroku-app-name&gt;.git</t>
   </si>
   <si>
+    <t xml:space="preserve">or link the Heroku existing app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git remote add heroku git.heroku.com/&lt;heroku-app-name&gt;.git</t>
+  </si>
+  <si>
     <t xml:space="preserve">New changes</t>
   </si>
   <si>
@@ -1272,6 +1285,44 @@
   </si>
   <si>
     <t xml:space="preserve">https://&lt;heroku-app-name&gt;.herokuapp.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssh: connect to host heroku.com port 22: Connection timed out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute heroku command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heroku git:remote -a &lt;app-name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fatal: remote heroku already exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open .git/config. Change &lt;app-name&gt; to the app name you want to push. Then</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[remote "heroku"]
+url = git@heroku.com:&lt;app-name&gt;.git
+fetch = +refs/heads/*:refs/remotes/heroku/*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Heroku app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git push heroku main/master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to link a folder with an existing Heroku app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link existing Heroku app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git remote add heroku git@heroku.com:project.git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Heroku app config</t>
   </si>
   <si>
     <t xml:space="preserve">Hardware</t>
@@ -1398,7 +1449,7 @@
     <numFmt numFmtId="169" formatCode="dd\-mm\-yyyy"/>
     <numFmt numFmtId="170" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1512,6 +1563,14 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1615,7 +1674,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1837,15 +1896,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1936,9 +2003,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
+      <xdr:colOff>262800</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>1988640</xdr:rowOff>
+      <xdr:rowOff>1986840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1952,7 +2019,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8393040" y="34497000"/>
-          <a:ext cx="9704160" cy="1950480"/>
+          <a:ext cx="9702360" cy="1948680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1973,9 +2040,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2655720</xdr:colOff>
+      <xdr:colOff>2653920</xdr:colOff>
       <xdr:row>128</xdr:row>
-      <xdr:rowOff>797760</xdr:rowOff>
+      <xdr:rowOff>795960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1989,7 +2056,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8481960" y="55080360"/>
-          <a:ext cx="2404440" cy="750240"/>
+          <a:ext cx="2402640" cy="748440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2015,9 +2082,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4580280</xdr:colOff>
+      <xdr:colOff>4578480</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>538560</xdr:rowOff>
+      <xdr:rowOff>536760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2031,7 +2098,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8477280" y="899640"/>
-          <a:ext cx="4333680" cy="448920"/>
+          <a:ext cx="4331880" cy="447120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2052,9 +2119,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4232160</xdr:colOff>
+      <xdr:colOff>4230360</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1664640</xdr:rowOff>
+      <xdr:rowOff>1662840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2068,7 +2135,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8337960" y="1536840"/>
-          <a:ext cx="4124880" cy="1632600"/>
+          <a:ext cx="4123080" cy="1630800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2089,9 +2156,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>5162400</xdr:colOff>
+      <xdr:colOff>5160600</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2105,7 +2172,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8436600" y="3497040"/>
-          <a:ext cx="4956480" cy="1472040"/>
+          <a:ext cx="4954680" cy="1470240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2126,9 +2193,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>754200</xdr:colOff>
+      <xdr:colOff>752400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1649520</xdr:rowOff>
+      <xdr:rowOff>1647720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2142,7 +2209,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8435160" y="5069520"/>
-          <a:ext cx="6392520" cy="1542960"/>
+          <a:ext cx="6390720" cy="1541160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2164,8 +2231,8 @@
   </sheetPr>
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3837,71 +3904,187 @@
       <c r="D48" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
+      <c r="H48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="14" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="J48" s="14" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="K48" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="L48" s="4" t="n">
         <f aca="false">L47+K48</f>
-        <v>57.275</v>
+        <v>60.275</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="21"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
+      <c r="A49" s="21" t="n">
+        <v>44737</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="14" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="J49" s="14" t="n">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="K49" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="L49" s="4" t="n">
         <f aca="false">L48+K49</f>
-        <v>57.275</v>
+        <v>65.275</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="21"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
+      <c r="A50" s="21" t="n">
+        <v>44740</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="14" t="n">
+        <v>0.361111111111111</v>
+      </c>
+      <c r="J50" s="14" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="K50" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L50" s="4" t="n">
+        <f aca="false">L49+K50</f>
+        <v>65.775</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="21"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
+      <c r="A51" s="21" t="n">
+        <v>44741</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" s="14" t="n">
+        <v>0.34375</v>
+      </c>
+      <c r="J51" s="14" t="n">
+        <v>0.381944444444444</v>
+      </c>
+      <c r="K51" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L51" s="4" t="n">
+        <f aca="false">L50+K51</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="21"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
+      <c r="L52" s="4" t="n">
+        <f aca="false">L51+K52</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="21"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
+      <c r="L53" s="4" t="n">
+        <f aca="false">L52+K53</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="21"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
+      <c r="L54" s="4" t="n">
+        <f aca="false">L53+K54</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="21"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
+      <c r="L55" s="4" t="n">
+        <f aca="false">L54+K55</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="21"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
+      <c r="L56" s="4" t="n">
+        <f aca="false">L55+K56</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="21"/>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
+      <c r="L57" s="4" t="n">
+        <f aca="false">L56+K57</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="21"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
+      <c r="L58" s="4" t="n">
+        <f aca="false">L57+K58</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="21"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
+      <c r="L59" s="4" t="n">
+        <f aca="false">L58+K59</f>
+        <v>66.775</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="21"/>
@@ -3943,9 +4126,278 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="42" width="78.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="65.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="39" width="10.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="40" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="54" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" s="59"/>
+    </row>
+    <row r="6" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>390</v>
+      </c>
+      <c r="D7" s="39" t="str">
+        <f aca="false">IF($D$3&lt;&gt;"","~/Documents/Ijps/Cursos/React","\React")</f>
+        <v>~/Documents/Ijps/Cursos/React</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="54" t="s">
+        <v>392</v>
+      </c>
+      <c r="D9" s="60" t="str">
+        <f aca="false">IF(D5&lt;&gt;"","N/A",IF(D6&lt;&gt;"","d:","N/A"))</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="54" t="s">
+        <v>393</v>
+      </c>
+      <c r="D10" s="60" t="str">
+        <f aca="false">_xlfn.CONCAT("cd ",$D$7)</f>
+        <v>cd ~/Documents/Ijps/Cursos/React</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="45"/>
+    </row>
+    <row r="12" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="41" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="54" t="s">
+        <v>395</v>
+      </c>
+      <c r="D13" s="60" t="str">
+        <f aca="false">_xlfn.CONCAT($D$10,"/",C13)</f>
+        <v>cd ~/Documents/Ijps/Cursos/React/fs-2021-examples</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="54" t="s">
+        <v>396</v>
+      </c>
+      <c r="D14" s="60" t="str">
+        <f aca="false">_xlfn.CONCAT($D$10,"/",C14)</f>
+        <v>cd ~/Documents/Ijps/Cursos/React/fs-2021</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="54" t="s">
+        <v>397</v>
+      </c>
+      <c r="D15" s="60" t="str">
+        <f aca="false">_xlfn.CONCAT($D$10,"/",C15)</f>
+        <v>cd ~/Documents/Ijps/Cursos/React/fs-2022-part3-phonebook-be</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="42"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="51"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="51"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="52"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="49"/>
+    </row>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -3960,16 +4412,16 @@
   <sheetData>
     <row r="1" s="40" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3977,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>382</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3985,57 +4437,57 @@
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>383</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="57" t="s">
-        <v>384</v>
+      <c r="C4" s="54" t="s">
+        <v>400</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>385</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="54.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="57" t="s">
-        <v>386</v>
+      <c r="C5" s="54" t="s">
+        <v>402</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="135.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="57" t="s">
-        <v>388</v>
+      <c r="C6" s="54" t="s">
+        <v>404</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="57" t="s">
-        <v>390</v>
+      <c r="C7" s="54" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="121.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="57" t="s">
-        <v>391</v>
+      <c r="C8" s="54" t="s">
+        <v>407</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>392</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="135.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="57" t="s">
-        <v>393</v>
+      <c r="C9" s="54" t="s">
+        <v>409</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="57" t="s">
-        <v>394</v>
+      <c r="C10" s="54" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4043,7 +4495,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>395</v>
+        <v>411</v>
       </c>
       <c r="D11" s="42"/>
     </row>
@@ -4052,10 +4504,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>396</v>
+        <v>412</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>397</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,7 +4521,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>398</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4077,10 +4529,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>399</v>
+        <v>415</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>400</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4122,14 +4574,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -4144,16 +4596,16 @@
   <sheetData>
     <row r="1" s="40" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4169,10 +4621,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>401</v>
+        <v>417</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>402</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4180,17 +4632,17 @@
         <v>2</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>403</v>
+        <v>419</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="57"/>
+      <c r="C5" s="54"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="57"/>
+      <c r="C6" s="54"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="42"/>
@@ -4339,7 +4791,7 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -4354,26 +4806,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D1" s="24" t="str">
         <f aca="false">C1</f>
-        <v>Part3c-2-Notes-BackEndToMongoDB</v>
+        <v>Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D2" s="24" t="str">
         <f aca="false">CONCATENATE(C1,"-", C2)</f>
-        <v>Part3c-2-Notes-BackEndToMongoDB-Development</v>
+        <v>Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1-Development</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4381,16 +4833,16 @@
     </row>
     <row r="4" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" s="27" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4398,7 +4850,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4406,7 +4858,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4414,11 +4866,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D7" s="28" t="str">
         <f aca="false">D1</f>
-        <v>Part3c-2-Notes-BackEndToMongoDB</v>
+        <v>Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4426,7 +4878,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" s="27" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4434,7 +4886,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4442,11 +4894,11 @@
         <v>1</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D12" s="22" t="str">
         <f aca="false">CONCATENATE("git checkout  -b ",$D$1)</f>
-        <v>git checkout  -b Part3c-2-Notes-BackEndToMongoDB</v>
+        <v>git checkout  -b Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4454,11 +4906,11 @@
         <v>2</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D13" s="22" t="str">
         <f aca="false">CONCATENATE("git fetch origin  ",$D$1)</f>
-        <v>git fetch origin  Part3c-2-Notes-BackEndToMongoDB</v>
+        <v>git fetch origin  Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4466,11 +4918,11 @@
         <v>3</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D14" s="22" t="str">
         <f aca="false">CONCATENATE("git pull origin  ",$D$1)</f>
-        <v>git pull origin  Part3c-2-Notes-BackEndToMongoDB</v>
+        <v>git pull origin  Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4478,107 +4930,107 @@
         <v>4</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D15" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="29"/>
       <c r="C16" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="29"/>
       <c r="C17" s="32" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="29"/>
       <c r="C18" s="32" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="29"/>
       <c r="C19" s="32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="29"/>
       <c r="C20" s="32" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="29"/>
       <c r="C21" s="33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="29"/>
       <c r="C22" s="35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="29"/>
       <c r="C23" s="33" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D23" s="34"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="29"/>
       <c r="C24" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="29"/>
       <c r="C25" s="33" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="29"/>
       <c r="C26" s="37" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="29"/>
       <c r="C27" s="38" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D27" s="29"/>
     </row>
@@ -4587,10 +5039,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4598,10 +5050,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4609,10 +5061,10 @@
         <v>5</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4620,11 +5072,11 @@
         <v>7</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D31" s="22" t="str">
         <f aca="false">CONCATENATE("git commit -m """,$D$2,"""")</f>
-        <v>git commit -m "Part3c-2-Notes-BackEndToMongoDB-Development"</v>
+        <v>git commit -m "Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1-Development"</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4632,11 +5084,11 @@
         <v>8</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D32" s="22" t="str">
         <f aca="false">CONCATENATE("git push origin  ",$D$1)</f>
-        <v>git push origin  Part3c-2-Notes-BackEndToMongoDB</v>
+        <v>git push origin  Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</v>
       </c>
     </row>
     <row r="35" s="27" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4644,7 +5096,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4652,10 +5104,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4663,10 +5115,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4674,10 +5126,10 @@
         <v>3</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4685,10 +5137,10 @@
         <v>4</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4696,11 +5148,11 @@
         <v>5</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D40" s="22" t="str">
         <f aca="false">CONCATENATE("git merge  ",$D$1)</f>
-        <v>git merge  Part3c-2-Notes-BackEndToMongoDB</v>
+        <v>git merge  Part3-3.13-PhoneBookBE-Step13-MongoDBToBackEndStep1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4708,10 +5160,10 @@
         <v>6</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4747,16 +5199,16 @@
   <sheetData>
     <row r="1" s="40" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4764,7 +5216,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4772,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4780,34 +5232,34 @@
         <v>2</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="39" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4815,7 +5267,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4823,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4831,10 +5283,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,10 +5294,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4853,10 +5305,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4864,18 +5316,18 @@
         <v>5</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="39" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4900,7 +5352,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.57"/>
@@ -4910,16 +5362,16 @@
   <sheetData>
     <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="27" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4927,7 +5379,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4935,7 +5387,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4943,10 +5395,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" s="27" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,7 +5406,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4962,7 +5414,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4970,10 +5422,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -5009,16 +5461,16 @@
   <sheetData>
     <row r="1" s="43" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="43" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="44" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5026,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,10 +5486,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5045,10 +5497,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5056,10 +5508,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" s="44" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5067,7 +5519,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5075,10 +5527,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5086,10 +5538,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5097,10 +5549,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" s="44" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5108,7 +5560,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5116,10 +5568,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" s="44" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5579,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5135,10 +5587,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,10 +5598,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,10 +5609,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -5196,16 +5648,16 @@
   <sheetData>
     <row r="1" s="40" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5213,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5221,7 +5673,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5229,10 +5681,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5243,7 +5695,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5251,7 +5703,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5259,10 +5711,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5270,10 +5722,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5426,7 +5878,7 @@
   </sheetPr>
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -5441,16 +5893,16 @@
   <sheetData>
     <row r="1" s="40" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5458,7 +5910,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5466,7 +5918,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5474,15 +5926,15 @@
         <v>2</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="42" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5490,7 +5942,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5498,7 +5950,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5506,41 +5958,41 @@
         <v>2</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="42" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="42" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="42" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="42" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="42" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5548,10 +6000,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5559,10 +6011,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5570,10 +6022,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5581,15 +6033,15 @@
         <v>6</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="39" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5597,26 +6049,26 @@
         <v>7</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="42" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="42" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5624,7 +6076,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5632,7 +6084,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5640,15 +6092,15 @@
         <v>2</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="42" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5656,7 +6108,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5664,7 +6116,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5672,15 +6124,15 @@
         <v>2</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="42" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5688,7 +6140,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5696,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5704,15 +6156,15 @@
         <v>2</v>
       </c>
       <c r="C39" s="42" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="42" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5720,15 +6172,15 @@
         <v>3</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="42" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5736,10 +6188,10 @@
         <v>4</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5747,7 +6199,7 @@
         <v>6</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5755,7 +6207,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5763,7 +6215,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5771,20 +6223,20 @@
         <v>3</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D49" s="39" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="42" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="42" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,7 +6244,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="44" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5800,7 +6252,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5808,15 +6260,15 @@
         <v>2</v>
       </c>
       <c r="C56" s="42" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D57" s="42" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5824,10 +6276,10 @@
         <v>3</v>
       </c>
       <c r="C58" s="42" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D58" s="39" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" s="41" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5835,10 +6287,10 @@
         <v>8</v>
       </c>
       <c r="C61" s="44" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D61" s="46" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5846,7 +6298,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5854,15 +6306,15 @@
         <v>2</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D64" s="42" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5870,10 +6322,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D65" s="42" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5881,10 +6333,10 @@
         <v>4</v>
       </c>
       <c r="C66" s="42" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D66" s="39" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5892,10 +6344,10 @@
         <v>5</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D67" s="39" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5903,10 +6355,10 @@
         <v>6</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D68" s="47" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5914,15 +6366,15 @@
         <v>7</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D69" s="39" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="42" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5930,10 +6382,10 @@
         <v>8</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D71" s="39" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5941,10 +6393,10 @@
         <v>9</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D72" s="39" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5952,10 +6404,10 @@
         <v>10</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D73" s="48" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5963,15 +6415,15 @@
         <v>11</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D74" s="39" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D75" s="42" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="78" s="41" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5979,10 +6431,10 @@
         <v>9</v>
       </c>
       <c r="C78" s="44" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D78" s="46" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5990,7 +6442,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,23 +6450,23 @@
         <v>2</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D80" s="39" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D81" s="42" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="42" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D82" s="42" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6022,10 +6474,10 @@
         <v>3</v>
       </c>
       <c r="C83" s="42" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D83" s="39" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6033,10 +6485,10 @@
         <v>4</v>
       </c>
       <c r="C84" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D84" s="42" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6044,18 +6496,18 @@
         <v>5</v>
       </c>
       <c r="C85" s="42" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D85" s="39" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="42" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D86" s="49" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="89" s="41" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6063,10 +6515,10 @@
         <v>10</v>
       </c>
       <c r="C89" s="44" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D89" s="46" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6074,7 +6526,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6082,18 +6534,18 @@
         <v>2</v>
       </c>
       <c r="C91" s="42" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D91" s="39" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="42" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D92" s="42" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="95" s="41" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6101,10 +6553,10 @@
         <v>11</v>
       </c>
       <c r="C95" s="44" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D95" s="46" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6112,7 +6564,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6120,10 +6572,10 @@
         <v>2</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D97" s="39" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6131,10 +6583,10 @@
         <v>3</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D98" s="42" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6142,10 +6594,10 @@
         <v>4</v>
       </c>
       <c r="C99" s="42" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D99" s="39" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6153,10 +6605,10 @@
         <v>5</v>
       </c>
       <c r="C100" s="42" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D100" s="50" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6164,15 +6616,15 @@
         <v>6</v>
       </c>
       <c r="C101" s="42" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D101" s="39" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D102" s="42" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6180,7 +6632,7 @@
         <v>7</v>
       </c>
       <c r="C103" s="42" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6188,10 +6640,10 @@
         <v>8</v>
       </c>
       <c r="C104" s="42" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D104" s="39" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" s="41" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6199,10 +6651,10 @@
         <v>11</v>
       </c>
       <c r="C107" s="44" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D107" s="46" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6210,7 +6662,7 @@
         <v>1</v>
       </c>
       <c r="C108" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6218,18 +6670,18 @@
         <v>2</v>
       </c>
       <c r="C109" s="42" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D109" s="39" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="42" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D110" s="42" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,15 +6689,15 @@
         <v>3</v>
       </c>
       <c r="C111" s="42" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D111" s="39" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D112" s="42" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6253,10 +6705,10 @@
         <v>4</v>
       </c>
       <c r="C113" s="42" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D113" s="39" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6264,10 +6716,10 @@
         <v>5</v>
       </c>
       <c r="C114" s="42" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D114" s="42" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6275,10 +6727,10 @@
         <v>6</v>
       </c>
       <c r="C115" s="42" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D115" s="42" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6286,7 +6738,7 @@
         <v>7</v>
       </c>
       <c r="C116" s="42" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6294,26 +6746,26 @@
         <v>8</v>
       </c>
       <c r="C117" s="42" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D117" s="39" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="42" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D118" s="39" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="42" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D119" s="39" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6321,7 +6773,7 @@
         <v>9</v>
       </c>
       <c r="C120" s="42" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6329,15 +6781,15 @@
         <v>10</v>
       </c>
       <c r="C121" s="42" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D121" s="39" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D122" s="42" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6345,15 +6797,15 @@
         <v>11</v>
       </c>
       <c r="C123" s="42" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D123" s="39" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D124" s="51" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6361,15 +6813,15 @@
         <v>12</v>
       </c>
       <c r="C125" s="42" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D125" s="39" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D126" s="51" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6377,10 +6829,10 @@
         <v>13</v>
       </c>
       <c r="C127" s="42" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D127" s="52" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6388,15 +6840,15 @@
         <v>14</v>
       </c>
       <c r="C128" s="42" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D128" s="39" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D129" s="49" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6421,10 +6873,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6438,16 +6890,16 @@
   <sheetData>
     <row r="1" s="40" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6455,7 +6907,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6463,7 +6915,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,7 +6923,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6479,10 +6931,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6490,7 +6942,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6498,10 +6950,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6509,10 +6961,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6520,10 +6972,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6531,10 +6983,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6542,89 +6994,89 @@
         <v>5</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="54" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="54" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="54" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="54" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="54" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="54" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="54" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="54" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="54" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="54" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="54" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6635,7 +7087,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6643,7 +7095,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6651,287 +7103,297 @@
         <v>2</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="54" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D29" s="45" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="54" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="32" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="41" t="n">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>366</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="41" t="n">
         <v>5</v>
       </c>
-      <c r="C32" s="44" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="39" t="n">
+      <c r="C33" s="44" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="42" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="39" t="n">
-        <v>2</v>
-      </c>
       <c r="C34" s="42" t="s">
-        <v>176</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>218</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="39" t="n">
         <v>4</v>
       </c>
-      <c r="C36" s="42" t="s">
-        <v>366</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="42"/>
-    </row>
-    <row r="38" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="41" t="n">
+      <c r="C37" s="42" t="s">
+        <v>370</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="42"/>
+    </row>
+    <row r="39" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="41" t="n">
         <v>6</v>
       </c>
-      <c r="C38" s="44" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="42" t="s">
-        <v>176</v>
+      <c r="C39" s="44" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="42" t="s">
         <v>205</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="39" t="n">
         <v>4</v>
       </c>
-      <c r="C42" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="D42" s="39" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="54" t="s">
-        <v>212</v>
+      <c r="C43" s="42" t="s">
+        <v>210</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="45" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="41" t="n">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="46" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="41" t="n">
         <v>7</v>
       </c>
-      <c r="C45" s="44" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" s="42" t="s">
-        <v>176</v>
+      <c r="C46" s="44" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="C47" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="D47" s="39" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="49" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="41" t="n">
+      <c r="C48" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" s="39" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="41" t="n">
         <v>8</v>
       </c>
-      <c r="C49" s="44" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="42" t="s">
-        <v>176</v>
+      <c r="C50" s="44" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="C51" s="42" t="s">
-        <v>222</v>
-      </c>
-      <c r="D51" s="39" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="39" t="n">
+      <c r="C52" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="C52" s="42" t="s">
-        <v>225</v>
-      </c>
-      <c r="D52" s="39" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="39" t="n">
+      <c r="C53" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="39" t="n">
         <v>4</v>
       </c>
-      <c r="C53" s="42" t="s">
-        <v>228</v>
-      </c>
-      <c r="D53" s="39" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="55" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="41" t="n">
+      <c r="C54" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="D54" s="39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="41" t="n">
         <v>9</v>
       </c>
-      <c r="C55" s="44" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="39" t="n">
+      <c r="C56" s="44" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="C56" s="42" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="39" t="n">
+      <c r="C57" s="42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="C57" s="42" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="39" t="n">
+      <c r="C58" s="42" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="C58" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="D58" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="41" t="n">
+      <c r="C59" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="D59" s="39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" s="41" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="41" t="n">
         <v>10</v>
       </c>
-      <c r="C60" s="44" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C61" s="42" t="s">
-        <v>176</v>
+      <c r="C61" s="44" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="C62" s="42" t="s">
-        <v>235</v>
-      </c>
-      <c r="D62" s="39" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="39" t="n">
+      <c r="C63" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="D63" s="39" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="C63" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="D63" s="39" t="s">
-        <v>239</v>
+      <c r="C64" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="D64" s="39" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D29" r:id="rId1" display="https://&lt;heroku-app-name&gt;.herokuapp.com"/>
-    <hyperlink ref="D30" r:id="rId2" display="https://git.heroku.com/&lt;heroku-app-name&gt;.git"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6950,8 +7412,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6965,139 +7427,102 @@
   <sheetData>
     <row r="1" s="40" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" s="56" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>369</v>
+      <c r="C2" s="57" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="55" t="s">
-        <v>370</v>
-      </c>
-      <c r="D3" s="56" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="55" t="s">
-        <v>372</v>
-      </c>
-      <c r="D4" s="56"/>
-    </row>
-    <row r="6" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="41" t="n">
+      <c r="C3" s="42" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" s="56" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="56" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>373</v>
+      <c r="C5" s="57" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="42" t="s">
+        <v>377</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="55" t="s">
-        <v>374</v>
-      </c>
-      <c r="D7" s="39" t="str">
-        <f aca="false">IF($D$3&lt;&gt;"","~/Documents/Ijps/Cursos/React","\React")</f>
-        <v>~/Documents/Ijps/Cursos/React</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="55" t="s">
+      <c r="C7" s="42" t="s">
+        <v>379</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="9" s="56" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="56" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="42" t="s">
+        <v>382</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="42" t="s">
+        <v>384</v>
+      </c>
+      <c r="D11" s="39" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="57" t="s">
-        <v>376</v>
-      </c>
-      <c r="D9" s="58" t="str">
-        <f aca="false">IF(D5&lt;&gt;"","N/A",IF(D6&lt;&gt;"","d:","N/A"))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="57" t="s">
-        <v>377</v>
-      </c>
-      <c r="D10" s="58" t="str">
-        <f aca="false">_xlfn.CONCAT("cd ",$D$7)</f>
-        <v>cd ~/Documents/Ijps/Cursos/React</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="45"/>
-    </row>
-    <row r="12" s="41" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="41" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="55" t="s">
-        <v>379</v>
-      </c>
-      <c r="D13" s="58" t="str">
-        <f aca="false">_xlfn.CONCAT($D$10,"/",C13)</f>
-        <v>cd ~/Documents/Ijps/Cursos/React/fs-2021-examples</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="55" t="s">
-        <v>380</v>
-      </c>
-      <c r="D14" s="58" t="str">
-        <f aca="false">_xlfn.CONCAT($D$10,"/",C14)</f>
-        <v>cd ~/Documents/Ijps/Cursos/React/fs-2021</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="55" t="s">
-        <v>381</v>
-      </c>
-      <c r="D15" s="58" t="str">
-        <f aca="false">_xlfn.CONCAT($D$10,"/",C15)</f>
-        <v>cd ~/Documents/Ijps/Cursos/React/fs-2022-part3-phonebook-be</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="42"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="51"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="51"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="52"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="49"/>
-    </row>
+    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7202,6 +7627,10 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" display="[remote &quot;heroku&quot;]&#10;url = git@heroku.com:&lt;app-name&gt;.git&#10;fetch = +refs/heads/*:refs/remotes/heroku/*"/>
+    <hyperlink ref="D10" r:id="rId2" display="git remote add heroku git@heroku.com:project.git"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>